<commit_message>
added new import files by using project
</commit_message>
<xml_diff>
--- a/public/IMPORT_TNVED_6302 (3).xlsx
+++ b/public/IMPORT_TNVED_6302 (3).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skiin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\web\job\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="225">
   <si>
     <t>Код ТНВЭД</t>
   </si>
@@ -695,21 +695,6 @@
   </si>
   <si>
     <t>Действие технических регламентов не распространяется</t>
-  </si>
-  <si>
-    <t>6302</t>
-  </si>
-  <si>
-    <t>Ивановский текстиль</t>
-  </si>
-  <si>
-    <t>100% Хлопок</t>
-  </si>
-  <si>
-    <t>6302100001</t>
-  </si>
-  <si>
-    <t>На модерации</t>
   </si>
 </sst>
 </file>
@@ -812,6 +797,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -822,7 +808,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1126,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B6" sqref="B5:B6"/>
+    <sheetView tabSelected="1" topLeftCell="G4" zoomScale="73" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N6" sqref="A5:N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1155,10 +1140,10 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="12" t="s">
         <v>3</v>
       </c>
       <c r="F1" s="2" t="s">
@@ -1202,10 +1187,10 @@
       <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="13" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
@@ -1332,61 +1317,16 @@
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>225</v>
-      </c>
       <c r="B5" s="7"/>
-      <c r="C5" t="s">
-        <v>226</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
       <c r="E5" s="7"/>
-      <c r="H5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J5" t="s">
-        <v>227</v>
-      </c>
       <c r="K5" s="9"/>
-      <c r="L5" t="s">
-        <v>228</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="N5" t="s">
-        <v>229</v>
-      </c>
+      <c r="M5" s="1"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>225</v>
-      </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
-      </c>
+      <c r="C6" s="1"/>
       <c r="E6" s="7"/>
-      <c r="H6" t="s">
-        <v>147</v>
-      </c>
-      <c r="J6" t="s">
-        <v>227</v>
-      </c>
-      <c r="L6" t="s">
-        <v>228</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="N6" t="s">
-        <v>229</v>
-      </c>
+      <c r="M6" s="1"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="10"/>
@@ -1406,7 +1346,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
-      <c r="B8" s="15"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="8"/>
@@ -1422,7 +1362,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
-      <c r="B9" s="15"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="8"/>
@@ -1514,10 +1454,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="14"/>
+      <c r="B1" s="15"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">

</xml_diff>